<commit_message>
add data to detail export
</commit_message>
<xml_diff>
--- a/dashboard/apps/prototype/templates/xls/ProjectDetail.xlsx
+++ b/dashboard/apps/prototype/templates/xls/ProjectDetail.xlsx
@@ -1,10 +1,10 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="25317"/>
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="26722"/>
   <workbookPr autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="3280" yWindow="680" windowWidth="25600" windowHeight="15620" tabRatio="500"/>
+    <workbookView xWindow="49100" yWindow="2720" windowWidth="25600" windowHeight="15620" tabRatio="500"/>
   </bookViews>
   <sheets>
     <sheet name="Crown Court Defence2 May16" sheetId="1" r:id="rId1"/>
@@ -944,10 +944,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:AF990"/>
+  <dimension ref="A1:AF988"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A10" sqref="A10:XFD19"/>
+      <selection activeCell="B22" sqref="B22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="13.5" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0"/>
@@ -1316,29 +1316,53 @@
       <c r="AE8" s="2"/>
       <c r="AF8" s="2"/>
     </row>
-    <row r="9" spans="1:32" ht="15" customHeight="1">
+    <row r="9" spans="1:32" ht="18" customHeight="1">
       <c r="A9" s="2"/>
       <c r="B9" s="2"/>
       <c r="C9" s="2"/>
       <c r="D9" s="2"/>
-      <c r="E9" s="24"/>
-      <c r="F9" s="24"/>
-      <c r="G9" s="24"/>
-      <c r="H9" s="24"/>
+      <c r="E9" s="2"/>
+      <c r="F9" s="2"/>
+      <c r="G9" s="2"/>
+      <c r="H9" s="2"/>
       <c r="I9" s="2"/>
-      <c r="J9" s="25"/>
-      <c r="K9" s="3"/>
-      <c r="L9" s="26"/>
-      <c r="M9" s="25"/>
-      <c r="N9" s="27"/>
+      <c r="J9" s="33">
+        <f>SUM(J7:J8)</f>
+        <v>0</v>
+      </c>
+      <c r="K9" s="34">
+        <f>SUM(K7:K8)</f>
+        <v>0</v>
+      </c>
+      <c r="L9" s="35"/>
+      <c r="M9" s="36"/>
+      <c r="N9" s="37">
+        <f>SUM(N7:N8)</f>
+        <v>10</v>
+      </c>
       <c r="O9" s="2"/>
       <c r="P9" s="2"/>
       <c r="Q9" s="2"/>
-      <c r="R9" s="28"/>
-      <c r="S9" s="29"/>
-      <c r="T9" s="29"/>
-      <c r="U9" s="29"/>
-      <c r="V9" s="30"/>
+      <c r="R9" s="38" t="e">
+        <f>SUM(#REF!)</f>
+        <v>#REF!</v>
+      </c>
+      <c r="S9" s="38" t="e">
+        <f>SUM(#REF!)</f>
+        <v>#REF!</v>
+      </c>
+      <c r="T9" s="38" t="e">
+        <f>SUM(#REF!)</f>
+        <v>#REF!</v>
+      </c>
+      <c r="U9" s="38" t="e">
+        <f>SUM(#REF!)</f>
+        <v>#REF!</v>
+      </c>
+      <c r="V9" s="38" t="e">
+        <f>SUM(#REF!)</f>
+        <v>#REF!</v>
+      </c>
       <c r="W9" s="2"/>
       <c r="X9" s="2"/>
       <c r="Y9" s="2"/>
@@ -1350,7 +1374,7 @@
       <c r="AE9" s="2"/>
       <c r="AF9" s="2"/>
     </row>
-    <row r="10" spans="1:32" ht="15.75" customHeight="1">
+    <row r="10" spans="1:32" ht="15" customHeight="1">
       <c r="A10" s="2"/>
       <c r="B10" s="2"/>
       <c r="C10" s="2"/>
@@ -1360,19 +1384,19 @@
       <c r="G10" s="2"/>
       <c r="H10" s="2"/>
       <c r="I10" s="2"/>
-      <c r="J10" s="25"/>
+      <c r="J10" s="3"/>
       <c r="K10" s="3"/>
-      <c r="L10" s="26"/>
-      <c r="M10" s="25"/>
-      <c r="N10" s="27"/>
+      <c r="L10" s="2"/>
+      <c r="M10" s="3"/>
+      <c r="N10" s="4"/>
       <c r="O10" s="2"/>
       <c r="P10" s="2"/>
       <c r="Q10" s="2"/>
-      <c r="R10" s="28"/>
-      <c r="S10" s="29"/>
-      <c r="T10" s="29"/>
-      <c r="U10" s="29"/>
-      <c r="V10" s="30"/>
+      <c r="R10" s="2"/>
+      <c r="S10" s="2"/>
+      <c r="T10" s="2"/>
+      <c r="U10" s="2"/>
+      <c r="V10" s="2"/>
       <c r="W10" s="2"/>
       <c r="X10" s="2"/>
       <c r="Y10" s="2"/>
@@ -1384,7 +1408,7 @@
       <c r="AE10" s="2"/>
       <c r="AF10" s="2"/>
     </row>
-    <row r="11" spans="1:32" ht="18" customHeight="1">
+    <row r="11" spans="1:32" ht="15" customHeight="1">
       <c r="A11" s="2"/>
       <c r="B11" s="2"/>
       <c r="C11" s="2"/>
@@ -1394,43 +1418,21 @@
       <c r="G11" s="2"/>
       <c r="H11" s="2"/>
       <c r="I11" s="2"/>
-      <c r="J11" s="33">
-        <f>SUM(J7:J10)</f>
-        <v>0</v>
+      <c r="J11" s="3"/>
+      <c r="K11" s="3"/>
+      <c r="L11" s="2"/>
+      <c r="M11" s="3"/>
+      <c r="N11" s="4"/>
+      <c r="O11" s="72" t="s">
+        <v>27</v>
       </c>
-      <c r="K11" s="34">
-        <f>SUM(K7:K10)</f>
-        <v>0</v>
-      </c>
-      <c r="L11" s="35"/>
-      <c r="M11" s="36"/>
-      <c r="N11" s="37">
-        <f>SUM(N7:N10)</f>
-        <v>10</v>
-      </c>
-      <c r="O11" s="2"/>
       <c r="P11" s="2"/>
       <c r="Q11" s="2"/>
-      <c r="R11" s="38">
-        <f>SUM(R10:R10)</f>
-        <v>0</v>
-      </c>
-      <c r="S11" s="38">
-        <f>SUM(S10:S10)</f>
-        <v>0</v>
-      </c>
-      <c r="T11" s="38">
-        <f>SUM(T10:T10)</f>
-        <v>0</v>
-      </c>
-      <c r="U11" s="38">
-        <f>SUM(U10:U10)</f>
-        <v>0</v>
-      </c>
-      <c r="V11" s="38">
-        <f>SUM(V10:V10)</f>
-        <v>0</v>
-      </c>
+      <c r="R11" s="2"/>
+      <c r="S11" s="2"/>
+      <c r="T11" s="2"/>
+      <c r="U11" s="2"/>
+      <c r="V11" s="2"/>
       <c r="W11" s="2"/>
       <c r="X11" s="2"/>
       <c r="Y11" s="2"/>
@@ -1455,9 +1457,14 @@
       <c r="J12" s="3"/>
       <c r="K12" s="3"/>
       <c r="L12" s="2"/>
-      <c r="M12" s="3"/>
-      <c r="N12" s="4"/>
-      <c r="O12" s="2"/>
+      <c r="M12" s="3" t="s">
+        <v>28</v>
+      </c>
+      <c r="N12" s="39" t="e">
+        <f>-SUM(N8+#REF!)</f>
+        <v>#REF!</v>
+      </c>
+      <c r="O12" s="68"/>
       <c r="P12" s="2"/>
       <c r="Q12" s="2"/>
       <c r="R12" s="2"/>
@@ -1476,7 +1483,7 @@
       <c r="AE12" s="2"/>
       <c r="AF12" s="2"/>
     </row>
-    <row r="13" spans="1:32" ht="15" customHeight="1">
+    <row r="13" spans="1:32" ht="15.75" customHeight="1">
       <c r="A13" s="2"/>
       <c r="B13" s="2"/>
       <c r="C13" s="2"/>
@@ -1490,10 +1497,8 @@
       <c r="K13" s="3"/>
       <c r="L13" s="2"/>
       <c r="M13" s="3"/>
-      <c r="N13" s="4"/>
-      <c r="O13" s="72" t="s">
-        <v>27</v>
-      </c>
+      <c r="N13" s="39"/>
+      <c r="O13" s="2"/>
       <c r="P13" s="2"/>
       <c r="Q13" s="2"/>
       <c r="R13" s="2"/>
@@ -1512,7 +1517,7 @@
       <c r="AE13" s="2"/>
       <c r="AF13" s="2"/>
     </row>
-    <row r="14" spans="1:32" ht="15" customHeight="1">
+    <row r="14" spans="1:32" ht="21" customHeight="1">
       <c r="A14" s="2"/>
       <c r="B14" s="2"/>
       <c r="C14" s="2"/>
@@ -1525,14 +1530,14 @@
       <c r="J14" s="3"/>
       <c r="K14" s="3"/>
       <c r="L14" s="2"/>
-      <c r="M14" s="3" t="s">
-        <v>28</v>
-      </c>
-      <c r="N14" s="39" t="e">
-        <f>-SUM(N8+#REF!)</f>
+      <c r="M14" s="3"/>
+      <c r="N14" s="40" t="e">
+        <f>SUM(N9:N13)</f>
         <v>#REF!</v>
       </c>
-      <c r="O14" s="68"/>
+      <c r="O14" s="2" t="s">
+        <v>29</v>
+      </c>
       <c r="P14" s="2"/>
       <c r="Q14" s="2"/>
       <c r="R14" s="2"/>
@@ -1551,7 +1556,7 @@
       <c r="AE14" s="2"/>
       <c r="AF14" s="2"/>
     </row>
-    <row r="15" spans="1:32" ht="15.75" customHeight="1">
+    <row r="15" spans="1:32" ht="15" customHeight="1">
       <c r="A15" s="2"/>
       <c r="B15" s="2"/>
       <c r="C15" s="2"/>
@@ -1565,7 +1570,7 @@
       <c r="K15" s="3"/>
       <c r="L15" s="2"/>
       <c r="M15" s="3"/>
-      <c r="N15" s="39"/>
+      <c r="N15" s="4"/>
       <c r="O15" s="2"/>
       <c r="P15" s="2"/>
       <c r="Q15" s="2"/>
@@ -1585,9 +1590,11 @@
       <c r="AE15" s="2"/>
       <c r="AF15" s="2"/>
     </row>
-    <row r="16" spans="1:32" ht="21" customHeight="1">
+    <row r="16" spans="1:32" ht="15" customHeight="1">
       <c r="A16" s="2"/>
-      <c r="B16" s="2"/>
+      <c r="B16" s="2" t="s">
+        <v>30</v>
+      </c>
       <c r="C16" s="2"/>
       <c r="D16" s="2"/>
       <c r="E16" s="2"/>
@@ -1599,13 +1606,8 @@
       <c r="K16" s="3"/>
       <c r="L16" s="2"/>
       <c r="M16" s="3"/>
-      <c r="N16" s="40" t="e">
-        <f>SUM(N11:N15)</f>
-        <v>#REF!</v>
-      </c>
-      <c r="O16" s="2" t="s">
-        <v>29</v>
-      </c>
+      <c r="N16" s="4"/>
+      <c r="O16" s="2"/>
       <c r="P16" s="2"/>
       <c r="Q16" s="2"/>
       <c r="R16" s="2"/>
@@ -1658,11 +1660,9 @@
       <c r="AE17" s="2"/>
       <c r="AF17" s="2"/>
     </row>
-    <row r="18" spans="1:32" ht="15" customHeight="1">
+    <row r="18" spans="1:32" ht="15.75" customHeight="1">
       <c r="A18" s="2"/>
-      <c r="B18" s="2" t="s">
-        <v>30</v>
-      </c>
+      <c r="B18" s="2"/>
       <c r="C18" s="2"/>
       <c r="D18" s="2"/>
       <c r="E18" s="2"/>
@@ -1706,13 +1706,15 @@
       <c r="I19" s="2"/>
       <c r="J19" s="3"/>
       <c r="K19" s="3"/>
-      <c r="L19" s="2"/>
-      <c r="M19" s="3"/>
-      <c r="N19" s="4"/>
-      <c r="O19" s="2"/>
-      <c r="P19" s="2"/>
-      <c r="Q19" s="2"/>
-      <c r="R19" s="2"/>
+      <c r="L19" s="41" t="s">
+        <v>31</v>
+      </c>
+      <c r="M19" s="42"/>
+      <c r="N19" s="43"/>
+      <c r="O19" s="44"/>
+      <c r="P19" s="42"/>
+      <c r="Q19" s="44"/>
+      <c r="R19" s="45"/>
       <c r="S19" s="2"/>
       <c r="T19" s="2"/>
       <c r="U19" s="2"/>
@@ -1728,7 +1730,7 @@
       <c r="AE19" s="2"/>
       <c r="AF19" s="2"/>
     </row>
-    <row r="20" spans="1:32" ht="15.75" customHeight="1">
+    <row r="20" spans="1:32" ht="15" customHeight="1">
       <c r="A20" s="2"/>
       <c r="B20" s="2"/>
       <c r="C20" s="2"/>
@@ -1740,13 +1742,13 @@
       <c r="I20" s="2"/>
       <c r="J20" s="3"/>
       <c r="K20" s="3"/>
-      <c r="L20" s="2"/>
-      <c r="M20" s="3"/>
-      <c r="N20" s="4"/>
-      <c r="O20" s="2"/>
-      <c r="P20" s="2"/>
-      <c r="Q20" s="2"/>
-      <c r="R20" s="2"/>
+      <c r="L20" s="46"/>
+      <c r="M20" s="47"/>
+      <c r="N20" s="48"/>
+      <c r="O20" s="49"/>
+      <c r="P20" s="47"/>
+      <c r="Q20" s="49"/>
+      <c r="R20" s="50"/>
       <c r="S20" s="2"/>
       <c r="T20" s="2"/>
       <c r="U20" s="2"/>
@@ -1774,15 +1776,13 @@
       <c r="I21" s="2"/>
       <c r="J21" s="3"/>
       <c r="K21" s="3"/>
-      <c r="L21" s="41" t="s">
-        <v>31</v>
-      </c>
-      <c r="M21" s="42"/>
-      <c r="N21" s="43"/>
-      <c r="O21" s="44"/>
-      <c r="P21" s="42"/>
-      <c r="Q21" s="44"/>
-      <c r="R21" s="45"/>
+      <c r="L21" s="46"/>
+      <c r="M21" s="47"/>
+      <c r="N21" s="48"/>
+      <c r="O21" s="49"/>
+      <c r="P21" s="47"/>
+      <c r="Q21" s="49"/>
+      <c r="R21" s="50"/>
       <c r="S21" s="2"/>
       <c r="T21" s="2"/>
       <c r="U21" s="2"/>
@@ -1798,7 +1798,7 @@
       <c r="AE21" s="2"/>
       <c r="AF21" s="2"/>
     </row>
-    <row r="22" spans="1:32" ht="15" customHeight="1">
+    <row r="22" spans="1:32" ht="17.25" customHeight="1">
       <c r="A22" s="2"/>
       <c r="B22" s="2"/>
       <c r="C22" s="2"/>
@@ -1810,10 +1810,14 @@
       <c r="I22" s="2"/>
       <c r="J22" s="3"/>
       <c r="K22" s="3"/>
-      <c r="L22" s="46"/>
-      <c r="M22" s="47"/>
-      <c r="N22" s="48"/>
-      <c r="O22" s="49"/>
+      <c r="L22" s="51" t="s">
+        <v>32</v>
+      </c>
+      <c r="M22" s="52"/>
+      <c r="N22" s="53"/>
+      <c r="O22" s="54" t="s">
+        <v>33</v>
+      </c>
       <c r="P22" s="47"/>
       <c r="Q22" s="49"/>
       <c r="R22" s="50"/>
@@ -1866,7 +1870,7 @@
       <c r="AE23" s="2"/>
       <c r="AF23" s="2"/>
     </row>
-    <row r="24" spans="1:32" ht="17.25" customHeight="1">
+    <row r="24" spans="1:32" ht="15" customHeight="1">
       <c r="A24" s="2"/>
       <c r="B24" s="2"/>
       <c r="C24" s="2"/>
@@ -1878,14 +1882,10 @@
       <c r="I24" s="2"/>
       <c r="J24" s="3"/>
       <c r="K24" s="3"/>
-      <c r="L24" s="51" t="s">
-        <v>32</v>
-      </c>
-      <c r="M24" s="52"/>
-      <c r="N24" s="53"/>
-      <c r="O24" s="54" t="s">
-        <v>33</v>
-      </c>
+      <c r="L24" s="46"/>
+      <c r="M24" s="47"/>
+      <c r="N24" s="48"/>
+      <c r="O24" s="49"/>
       <c r="P24" s="47"/>
       <c r="Q24" s="49"/>
       <c r="R24" s="50"/>
@@ -1919,7 +1919,7 @@
       <c r="L25" s="46"/>
       <c r="M25" s="47"/>
       <c r="N25" s="48"/>
-      <c r="O25" s="49"/>
+      <c r="O25" s="55"/>
       <c r="P25" s="47"/>
       <c r="Q25" s="49"/>
       <c r="R25" s="50"/>
@@ -1952,11 +1952,16 @@
       <c r="K26" s="3"/>
       <c r="L26" s="46"/>
       <c r="M26" s="47"/>
-      <c r="N26" s="48"/>
-      <c r="O26" s="49"/>
+      <c r="N26" s="48" t="s">
+        <v>34</v>
+      </c>
+      <c r="O26" s="55" t="e">
+        <f>#REF!+#REF!</f>
+        <v>#REF!</v>
+      </c>
       <c r="P26" s="47"/>
-      <c r="Q26" s="49"/>
-      <c r="R26" s="50"/>
+      <c r="Q26" s="55"/>
+      <c r="R26" s="56"/>
       <c r="S26" s="2"/>
       <c r="T26" s="2"/>
       <c r="U26" s="2"/>
@@ -1984,13 +1989,20 @@
       <c r="I27" s="2"/>
       <c r="J27" s="3"/>
       <c r="K27" s="3"/>
-      <c r="L27" s="46"/>
-      <c r="M27" s="47"/>
-      <c r="N27" s="48"/>
-      <c r="O27" s="55"/>
-      <c r="P27" s="47"/>
-      <c r="Q27" s="49"/>
-      <c r="R27" s="50"/>
+      <c r="L27" s="57"/>
+      <c r="M27" s="58"/>
+      <c r="N27" s="48" t="s">
+        <v>35</v>
+      </c>
+      <c r="O27" s="59" t="e">
+        <f>#REF!+#REF!</f>
+        <v>#REF!</v>
+      </c>
+      <c r="P27" s="73" t="s">
+        <v>36</v>
+      </c>
+      <c r="Q27" s="68"/>
+      <c r="R27" s="74"/>
       <c r="S27" s="2"/>
       <c r="T27" s="2"/>
       <c r="U27" s="2"/>
@@ -2018,13 +2030,11 @@
       <c r="I28" s="2"/>
       <c r="J28" s="3"/>
       <c r="K28" s="3"/>
-      <c r="L28" s="46"/>
-      <c r="M28" s="47"/>
-      <c r="N28" s="48" t="s">
-        <v>34</v>
-      </c>
-      <c r="O28" s="55" t="e">
-        <f>#REF!+#REF!</f>
+      <c r="L28" s="57"/>
+      <c r="M28" s="58"/>
+      <c r="N28" s="48"/>
+      <c r="O28" s="60" t="e">
+        <f>SUM(O26:O27)</f>
         <v>#REF!</v>
       </c>
       <c r="P28" s="47"/>
@@ -2045,7 +2055,7 @@
       <c r="AE28" s="2"/>
       <c r="AF28" s="2"/>
     </row>
-    <row r="29" spans="1:32" ht="15" customHeight="1">
+    <row r="29" spans="1:32" ht="15.75" customHeight="1">
       <c r="A29" s="2"/>
       <c r="B29" s="2"/>
       <c r="C29" s="2"/>
@@ -2057,20 +2067,13 @@
       <c r="I29" s="2"/>
       <c r="J29" s="3"/>
       <c r="K29" s="3"/>
-      <c r="L29" s="57"/>
-      <c r="M29" s="58"/>
-      <c r="N29" s="48" t="s">
-        <v>35</v>
-      </c>
-      <c r="O29" s="59" t="e">
-        <f>#REF!+#REF!</f>
-        <v>#REF!</v>
-      </c>
-      <c r="P29" s="73" t="s">
-        <v>36</v>
-      </c>
-      <c r="Q29" s="68"/>
-      <c r="R29" s="74"/>
+      <c r="L29" s="61"/>
+      <c r="M29" s="62"/>
+      <c r="N29" s="63"/>
+      <c r="O29" s="64"/>
+      <c r="P29" s="65"/>
+      <c r="Q29" s="64"/>
+      <c r="R29" s="66"/>
       <c r="S29" s="2"/>
       <c r="T29" s="2"/>
       <c r="U29" s="2"/>
@@ -2086,7 +2089,7 @@
       <c r="AE29" s="2"/>
       <c r="AF29" s="2"/>
     </row>
-    <row r="30" spans="1:32" ht="15" customHeight="1">
+    <row r="30" spans="1:32">
       <c r="A30" s="2"/>
       <c r="B30" s="2"/>
       <c r="C30" s="2"/>
@@ -2098,16 +2101,13 @@
       <c r="I30" s="2"/>
       <c r="J30" s="3"/>
       <c r="K30" s="3"/>
-      <c r="L30" s="57"/>
-      <c r="M30" s="58"/>
-      <c r="N30" s="48"/>
-      <c r="O30" s="60" t="e">
-        <f>SUM(O28:O29)</f>
-        <v>#REF!</v>
-      </c>
-      <c r="P30" s="47"/>
-      <c r="Q30" s="55"/>
-      <c r="R30" s="56"/>
+      <c r="L30" s="2"/>
+      <c r="M30" s="3"/>
+      <c r="N30" s="4"/>
+      <c r="O30" s="2"/>
+      <c r="P30" s="2"/>
+      <c r="Q30" s="2"/>
+      <c r="R30" s="2"/>
       <c r="S30" s="2"/>
       <c r="T30" s="2"/>
       <c r="U30" s="2"/>
@@ -2123,7 +2123,7 @@
       <c r="AE30" s="2"/>
       <c r="AF30" s="2"/>
     </row>
-    <row r="31" spans="1:32" ht="15.75" customHeight="1">
+    <row r="31" spans="1:32">
       <c r="A31" s="2"/>
       <c r="B31" s="2"/>
       <c r="C31" s="2"/>
@@ -2135,13 +2135,13 @@
       <c r="I31" s="2"/>
       <c r="J31" s="3"/>
       <c r="K31" s="3"/>
-      <c r="L31" s="61"/>
-      <c r="M31" s="62"/>
-      <c r="N31" s="63"/>
-      <c r="O31" s="64"/>
-      <c r="P31" s="65"/>
-      <c r="Q31" s="64"/>
-      <c r="R31" s="66"/>
+      <c r="L31" s="2"/>
+      <c r="M31" s="3"/>
+      <c r="N31" s="4"/>
+      <c r="O31" s="2"/>
+      <c r="P31" s="2"/>
+      <c r="Q31" s="2"/>
+      <c r="R31" s="2"/>
       <c r="S31" s="2"/>
       <c r="T31" s="2"/>
       <c r="U31" s="2"/>
@@ -34695,80 +34695,12 @@
       <c r="AE988" s="2"/>
       <c r="AF988" s="2"/>
     </row>
-    <row r="989" spans="1:32">
-      <c r="A989" s="2"/>
-      <c r="B989" s="2"/>
-      <c r="C989" s="2"/>
-      <c r="D989" s="2"/>
-      <c r="E989" s="2"/>
-      <c r="F989" s="2"/>
-      <c r="G989" s="2"/>
-      <c r="H989" s="2"/>
-      <c r="I989" s="2"/>
-      <c r="J989" s="3"/>
-      <c r="K989" s="3"/>
-      <c r="L989" s="2"/>
-      <c r="M989" s="3"/>
-      <c r="N989" s="4"/>
-      <c r="O989" s="2"/>
-      <c r="P989" s="2"/>
-      <c r="Q989" s="2"/>
-      <c r="R989" s="2"/>
-      <c r="S989" s="2"/>
-      <c r="T989" s="2"/>
-      <c r="U989" s="2"/>
-      <c r="V989" s="2"/>
-      <c r="W989" s="2"/>
-      <c r="X989" s="2"/>
-      <c r="Y989" s="2"/>
-      <c r="Z989" s="2"/>
-      <c r="AA989" s="2"/>
-      <c r="AB989" s="2"/>
-      <c r="AC989" s="2"/>
-      <c r="AD989" s="2"/>
-      <c r="AE989" s="2"/>
-      <c r="AF989" s="2"/>
-    </row>
-    <row r="990" spans="1:32">
-      <c r="A990" s="2"/>
-      <c r="B990" s="2"/>
-      <c r="C990" s="2"/>
-      <c r="D990" s="2"/>
-      <c r="E990" s="2"/>
-      <c r="F990" s="2"/>
-      <c r="G990" s="2"/>
-      <c r="H990" s="2"/>
-      <c r="I990" s="2"/>
-      <c r="J990" s="3"/>
-      <c r="K990" s="3"/>
-      <c r="L990" s="2"/>
-      <c r="M990" s="3"/>
-      <c r="N990" s="4"/>
-      <c r="O990" s="2"/>
-      <c r="P990" s="2"/>
-      <c r="Q990" s="2"/>
-      <c r="R990" s="2"/>
-      <c r="S990" s="2"/>
-      <c r="T990" s="2"/>
-      <c r="U990" s="2"/>
-      <c r="V990" s="2"/>
-      <c r="W990" s="2"/>
-      <c r="X990" s="2"/>
-      <c r="Y990" s="2"/>
-      <c r="Z990" s="2"/>
-      <c r="AA990" s="2"/>
-      <c r="AB990" s="2"/>
-      <c r="AC990" s="2"/>
-      <c r="AD990" s="2"/>
-      <c r="AE990" s="2"/>
-      <c r="AF990" s="2"/>
-    </row>
   </sheetData>
   <mergeCells count="4">
     <mergeCell ref="D2:N2"/>
     <mergeCell ref="G3:M3"/>
-    <mergeCell ref="O13:O14"/>
-    <mergeCell ref="P29:R29"/>
+    <mergeCell ref="O11:O12"/>
+    <mergeCell ref="P27:R27"/>
   </mergeCells>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
   <extLst>

</xml_diff>

<commit_message>
remove custom client from project detail xlsx template
</commit_message>
<xml_diff>
--- a/dashboard/apps/prototype/templates/xls/ProjectDetail.xlsx
+++ b/dashboard/apps/prototype/templates/xls/ProjectDetail.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="26722"/>
   <workbookPr autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="49100" yWindow="2720" windowWidth="25600" windowHeight="15620" tabRatio="500"/>
+    <workbookView xWindow="38620" yWindow="3320" windowWidth="25600" windowHeight="15620" tabRatio="500"/>
   </bookViews>
   <sheets>
     <sheet name="Crown Court Defence2 May16" sheetId="1" r:id="rId1"/>
@@ -102,25 +102,7 @@
     <t>to be confirmed</t>
   </si>
   <si>
-    <t>LAA Payroll costs already incurred</t>
-  </si>
-  <si>
     <t xml:space="preserve">LESS </t>
-  </si>
-  <si>
-    <t>RECHARGED to LAA</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Recharge Arrangement agreed for May 16 is for 5 Team members on this project, to be recharged 100% to LAA </t>
-  </si>
-  <si>
-    <t>Project Costs - 100% to LAA for May 16</t>
-  </si>
-  <si>
-    <t>to be Recharged to LAA - P2 May 16</t>
-  </si>
-  <si>
-    <t>ours + LAA payroll charges</t>
   </si>
   <si>
     <t>Agency</t>
@@ -129,10 +111,28 @@
     <t>Salaried</t>
   </si>
   <si>
-    <t xml:space="preserve">MoJ; LAA Payroll costs incurred directly </t>
+    <t>Project: name</t>
   </si>
   <si>
-    <t>Project: name</t>
+    <t xml:space="preserve">Recharge Arrangement agreed for #PERIOD is for#NUMBER_TEAM_MEMBERS Team members on this project, to be recharged 100% to #CLIENT </t>
+  </si>
+  <si>
+    <t>Project Costs - 100% to #CLIENT for #PERIOD</t>
+  </si>
+  <si>
+    <t>to be Recharged to #CLIENT - P2 #PERIOD</t>
+  </si>
+  <si>
+    <t>ours + #CLIENT payroll charges</t>
+  </si>
+  <si>
+    <t>RECHARGED to #CLIENT</t>
+  </si>
+  <si>
+    <t>#CLIENT Payroll costs already incurred</t>
+  </si>
+  <si>
+    <t xml:space="preserve">MoJ - #CLIENT Payroll costs incurred directly </t>
   </si>
 </sst>
 </file>
@@ -946,8 +946,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:AF988"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B22" sqref="B22"/>
+    <sheetView tabSelected="1" topLeftCell="C1" workbookViewId="0">
+      <selection activeCell="S32" sqref="S32"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="13.5" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0"/>
@@ -1080,7 +1080,7 @@
     </row>
     <row r="4" spans="1:32" ht="15" customHeight="1">
       <c r="A4" s="6" t="s">
-        <v>37</v>
+        <v>30</v>
       </c>
       <c r="B4" s="6"/>
       <c r="C4" s="6"/>
@@ -1424,7 +1424,7 @@
       <c r="M11" s="3"/>
       <c r="N11" s="4"/>
       <c r="O11" s="72" t="s">
-        <v>27</v>
+        <v>36</v>
       </c>
       <c r="P11" s="2"/>
       <c r="Q11" s="2"/>
@@ -1458,7 +1458,7 @@
       <c r="K12" s="3"/>
       <c r="L12" s="2"/>
       <c r="M12" s="3" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="N12" s="39" t="e">
         <f>-SUM(N8+#REF!)</f>
@@ -1536,7 +1536,7 @@
         <v>#REF!</v>
       </c>
       <c r="O14" s="2" t="s">
-        <v>29</v>
+        <v>35</v>
       </c>
       <c r="P14" s="2"/>
       <c r="Q14" s="2"/>
@@ -1593,7 +1593,7 @@
     <row r="16" spans="1:32" ht="15" customHeight="1">
       <c r="A16" s="2"/>
       <c r="B16" s="2" t="s">
-        <v>30</v>
+        <v>31</v>
       </c>
       <c r="C16" s="2"/>
       <c r="D16" s="2"/>
@@ -1707,7 +1707,7 @@
       <c r="J19" s="3"/>
       <c r="K19" s="3"/>
       <c r="L19" s="41" t="s">
-        <v>31</v>
+        <v>32</v>
       </c>
       <c r="M19" s="42"/>
       <c r="N19" s="43"/>
@@ -1811,12 +1811,12 @@
       <c r="J22" s="3"/>
       <c r="K22" s="3"/>
       <c r="L22" s="51" t="s">
-        <v>32</v>
+        <v>33</v>
       </c>
       <c r="M22" s="52"/>
       <c r="N22" s="53"/>
       <c r="O22" s="54" t="s">
-        <v>33</v>
+        <v>34</v>
       </c>
       <c r="P22" s="47"/>
       <c r="Q22" s="49"/>
@@ -1953,7 +1953,7 @@
       <c r="L26" s="46"/>
       <c r="M26" s="47"/>
       <c r="N26" s="48" t="s">
-        <v>34</v>
+        <v>28</v>
       </c>
       <c r="O26" s="55" t="e">
         <f>#REF!+#REF!</f>
@@ -1992,14 +1992,14 @@
       <c r="L27" s="57"/>
       <c r="M27" s="58"/>
       <c r="N27" s="48" t="s">
-        <v>35</v>
+        <v>29</v>
       </c>
       <c r="O27" s="59" t="e">
         <f>#REF!+#REF!</f>
         <v>#REF!</v>
       </c>
       <c r="P27" s="73" t="s">
-        <v>36</v>
+        <v>37</v>
       </c>
       <c r="Q27" s="68"/>
       <c r="R27" s="74"/>

</xml_diff>